<commit_message>
Enhancements: Single login hook, increased test coverage, minor code tweaks
</commit_message>
<xml_diff>
--- a/Testing_Artifacts/3. Manual TC, bug reports, screenshots/Test Cases and Bug Reports.xlsx
+++ b/Testing_Artifacts/3. Manual TC, bug reports, screenshots/Test Cases and Bug Reports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissakanyi/Desktop/Incourage Project Deliverables/Manual TC, bug reports, screenshots/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melissakanyi/Downloads/Loan-Management-System-master/Testing_Artifacts/3. Manual TC, bug reports, screenshots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F6851D-DD15-C04D-A554-18B3029FA34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B05F42-0C16-444B-90DB-2856EF4145F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="700" yWindow="500" windowWidth="35500" windowHeight="18840" activeTab="2" xr2:uid="{82C73610-8692-264B-8B7B-EB74EAB39CC4}"/>
+    <workbookView xWindow="700" yWindow="500" windowWidth="35500" windowHeight="18840" activeTab="1" xr2:uid="{82C73610-8692-264B-8B7B-EB74EAB39CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="179">
   <si>
     <t>Test Case</t>
   </si>
@@ -646,6 +646,27 @@
   </si>
   <si>
     <t>Fix errors DB inorder to connect</t>
+  </si>
+  <si>
+    <t>Duplicate contacts</t>
+  </si>
+  <si>
+    <t>BG-DC-01</t>
+  </si>
+  <si>
+    <t>allClients</t>
+  </si>
+  <si>
+    <t>Contacts have no unique identifiers so Admins can create multiple contacts</t>
+  </si>
+  <si>
+    <t>1. In the borrower's page create a client contact by filling out all required fields
+2. Create another new contact with the same fields
+3.Duplicate contacts are created with the same details</t>
+  </si>
+  <si>
+    <t>Cypress
+Firefox browser</t>
   </si>
 </sst>
 </file>
@@ -773,12 +794,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -794,6 +809,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,8 +1152,8 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1152,11 +1173,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -1164,56 +1185,56 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-    </row>
-    <row r="6" spans="1:11" s="16" customFormat="1" ht="23">
-      <c r="A6" s="16" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+    </row>
+    <row r="6" spans="1:11" s="14" customFormat="1" ht="23">
+      <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="E6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="J6" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="18" t="s">
+      <c r="K6" s="16" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="114" customHeight="1">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
       <c r="B7" s="7" t="s">
@@ -1248,7 +1269,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="84" customHeight="1">
-      <c r="A8" s="12"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="7" t="s">
         <v>53</v>
       </c>
@@ -1638,11 +1659,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EF3EB6-FC6A-E949-86F0-0EB9202BD703}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1656,38 +1677,38 @@
     <col min="12" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="14" customFormat="1" ht="47" customHeight="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:11" s="12" customFormat="1" ht="47" customHeight="1">
+      <c r="A1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="13" t="s">
         <v>116</v>
       </c>
     </row>
@@ -1861,6 +1882,38 @@
         <v>124</v>
       </c>
       <c r="K6" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="51">
+      <c r="A7" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="K7" s="11" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1873,7 +1926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D068C45-11E8-C64F-9A64-D975A6E8C46F}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
@@ -1882,27 +1935,27 @@
   <cols>
     <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="3" width="64.5" style="20" customWidth="1"/>
+    <col min="3" max="3" width="64.5" style="18" customWidth="1"/>
     <col min="4" max="4" width="80" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-    </row>
-    <row r="2" spans="1:4" s="19" customFormat="1" ht="22" customHeight="1">
-      <c r="B2" s="19" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+    </row>
+    <row r="2" spans="1:4" s="17" customFormat="1" ht="22" customHeight="1">
+      <c r="B2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="17" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1910,7 +1963,7 @@
       <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>171</v>
       </c>
       <c r="D3" t="s">
@@ -1921,7 +1974,7 @@
       <c r="B4" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>172</v>
       </c>
       <c r="D4" t="s">
@@ -1932,7 +1985,7 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="18" t="s">
         <v>97</v>
       </c>
       <c r="D5" t="s">
@@ -1940,17 +1993,17 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="18" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="18" t="s">
         <v>98</v>
       </c>
     </row>

</xml_diff>